<commit_message>
small changes to rf calculation
</commit_message>
<xml_diff>
--- a/Session 5/ReceptiveField_Calculation.xlsx
+++ b/Session 5/ReceptiveField_Calculation.xlsx
@@ -617,7 +617,7 @@
   <dimension ref="A2:R52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1064,8 +1064,7 @@
         <v>14</v>
       </c>
       <c r="M22" s="0" t="n">
-        <f aca="false">CNN[[#This Row],[rin]]+(CNN[[#This Row],[kernel]]-1)*CNN[[#This Row],[jin]]</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N22" s="0" t="n">
         <f aca="false">(CNN[[#This Row],[nin]]*CNN[[#This Row],[nin]]*CNN[[#This Row],[Channels]])</f>
@@ -1118,11 +1117,11 @@
       </c>
       <c r="L23" s="0" t="n">
         <f aca="false">M22</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M23" s="0" t="n">
         <f aca="false">CNN[[#This Row],[rin]]+(CNN[[#This Row],[kernel]]-1)*CNN[[#This Row],[jin]]</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N23" s="0" t="n">
         <f aca="false">(CNN[[#This Row],[nin]]*CNN[[#This Row],[nin]]*CNN[[#This Row],[Channels]])</f>
@@ -1170,11 +1169,11 @@
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">M23</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M24" s="0" t="n">
         <f aca="false">CNN[[#This Row],[rin]]+(CNN[[#This Row],[kernel]]-1)*CNN[[#This Row],[jin]]</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N24" s="0" t="n">
         <f aca="false">(CNN[[#This Row],[nin]]*CNN[[#This Row],[nin]]*CNN[[#This Row],[Channels]])</f>
@@ -1218,10 +1217,10 @@
         <v>2</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N25" s="0" t="n">
         <f aca="false">(CNN[[#This Row],[nin]]*CNN[[#This Row],[nin]]*CNN[[#This Row],[Channels]])</f>

</xml_diff>